<commit_message>
2nd commit from Cyan
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lixil/Documents/GitHub/FirstRepoTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D731E38E-1A84-0344-88AF-458A2A6F1EC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED25A48-56C3-4C48-AE41-0F5B8C55E880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{898A2C00-0DC0-C944-9A36-C571DCFDC79F}"/>
   </bookViews>
@@ -379,17 +379,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2B9BAD-E379-0B4C-AEDE-08D694169C9F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>111</v>
+      </c>
+      <c r="B1">
+        <v>666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>